<commit_message>
updated status for state outreach
</commit_message>
<xml_diff>
--- a/#State Mapping Status.xlsx
+++ b/#State Mapping Status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="30760" yWindow="-1440" windowWidth="32980" windowHeight="16640"/>
+    <workbookView xWindow="30380" yWindow="-2040" windowWidth="33660" windowHeight="20560"/>
   </bookViews>
   <sheets>
     <sheet name="SEARCH" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="139">
   <si>
     <t>State</t>
   </si>
@@ -107,9 +107,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Alabama</t>
   </si>
   <si>
@@ -284,9 +281,6 @@
     <t>Mike Lesko</t>
   </si>
   <si>
-    <t xml:space="preserve">NCIC code </t>
-  </si>
-  <si>
     <t>Captain John Rattigan</t>
   </si>
   <si>
@@ -320,12 +314,6 @@
     <t>Leslie Moore</t>
   </si>
   <si>
-    <t>Dana Gotz</t>
-  </si>
-  <si>
-    <t>Patricia Zafke</t>
-  </si>
-  <si>
     <t>Bob Merwine</t>
   </si>
   <si>
@@ -353,9 +341,6 @@
     <t>Major David Flannian</t>
   </si>
   <si>
-    <t>interested in assistance with mapping</t>
-  </si>
-  <si>
     <t>Sam Clark</t>
   </si>
   <si>
@@ -390,13 +375,85 @@
   </si>
   <si>
     <t>only statute and NCIC code included in table (not very good mappings)</t>
+  </si>
+  <si>
+    <t>Matt Ruel</t>
+  </si>
+  <si>
+    <t>Andrew to contact</t>
+  </si>
+  <si>
+    <t>Jeff Wallin</t>
+  </si>
+  <si>
+    <t>Brad Truitt</t>
+  </si>
+  <si>
+    <t>Chad Mosteller</t>
+  </si>
+  <si>
+    <t>Rickeya Franklin</t>
+  </si>
+  <si>
+    <t>Brandon Gray</t>
+  </si>
+  <si>
+    <t>Jeff Kellett</t>
+  </si>
+  <si>
+    <t>Curt Wood</t>
+  </si>
+  <si>
+    <t>Lt. Col. Timothy Chung</t>
+  </si>
+  <si>
+    <t>Chris Andrist</t>
+  </si>
+  <si>
+    <t>Michael Lawlor</t>
+  </si>
+  <si>
+    <t>Lisa Seymour</t>
+  </si>
+  <si>
+    <t>Chris Young</t>
+  </si>
+  <si>
+    <t>Becki contacted Mannone Butler (SEARCH member) and she is following up on the request</t>
+  </si>
+  <si>
+    <t>Need to contact</t>
+  </si>
+  <si>
+    <t>Becki contacted on 3/13</t>
+  </si>
+  <si>
+    <t>Maping received after Becki followed up on 3/13</t>
+  </si>
+  <si>
+    <t>Becki followed up on 3/13 - no mapping available</t>
+  </si>
+  <si>
+    <t>Becki contacted on 3/13 - Mr. Wood is following up</t>
+  </si>
+  <si>
+    <t>need to create mapping</t>
+  </si>
+  <si>
+    <t>Dana Gotz/Patrici Zafke</t>
+  </si>
+  <si>
+    <t>interested in assistance with mapping - need to create mapping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Becki contacted on 3/13 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,12 +475,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -437,13 +488,37 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -455,12 +530,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -485,12 +562,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -774,7 +858,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J31" sqref="J31"/>
+      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -822,9 +906,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -844,14 +928,17 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>135</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -871,17 +958,17 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -894,12 +981,18 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
+      <c r="I4" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>130</v>
+      </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -919,14 +1012,14 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -940,20 +1033,21 @@
       <c r="E6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>135</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
@@ -966,12 +1060,18 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
+      <c r="I7" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>130</v>
+      </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
@@ -984,12 +1084,18 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
+      <c r="I8" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>130</v>
+      </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>4</v>
@@ -1002,12 +1108,18 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
+      <c r="I9" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>130</v>
+      </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
@@ -1027,17 +1139,17 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
@@ -1053,9 +1165,9 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>4</v>
@@ -1067,12 +1179,18 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="H12" s="2"/>
+      <c r="I12" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>131</v>
+      </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>4</v>
@@ -1091,17 +1209,17 @@
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>119</v>
+        <v>106</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>4</v>
@@ -1115,19 +1233,20 @@
       <c r="E14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="F14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>135</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>4</v>
@@ -1141,19 +1260,20 @@
       <c r="E15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="F15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>135</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>4</v>
@@ -1172,17 +1292,17 @@
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>4</v>
@@ -1201,14 +1321,14 @@
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>4</v>
@@ -1222,19 +1342,20 @@
       <c r="E18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="F18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>135</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>4</v>
@@ -1246,12 +1367,18 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="H19" s="2"/>
+      <c r="I19" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>116</v>
+      </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>4</v>
@@ -1265,19 +1392,20 @@
       <c r="E20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="F20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>135</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>4</v>
@@ -1289,12 +1417,18 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="H21" s="2"/>
+      <c r="I21" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>134</v>
+      </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>4</v>
@@ -1313,14 +1447,14 @@
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>4</v>
@@ -1339,17 +1473,14 @@
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>97</v>
+        <v>136</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>4</v>
@@ -1363,22 +1494,20 @@
       <c r="E24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="F24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>137</v>
       </c>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>4</v>
@@ -1397,14 +1526,14 @@
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>4</v>
@@ -1423,14 +1552,14 @@
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>4</v>
@@ -1449,14 +1578,14 @@
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>4</v>
@@ -1468,12 +1597,18 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="H28" s="2"/>
+      <c r="I28" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>130</v>
+      </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>4</v>
@@ -1481,16 +1616,28 @@
       <c r="C29" s="3">
         <v>43102</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="D29" s="3">
+        <v>43172</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H29" s="2"/>
+      <c r="I29" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>132</v>
+      </c>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>4</v>
@@ -1509,17 +1656,17 @@
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>4</v>
@@ -1533,22 +1680,20 @@
       <c r="E31" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="F31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>107</v>
+        <v>95</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>137</v>
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>4</v>
@@ -1567,17 +1712,17 @@
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="J32" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>99</v>
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
     <row r="33" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>4</v>
@@ -1585,17 +1730,26 @@
       <c r="C33" s="3">
         <v>43102</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="2"/>
+      <c r="D33" s="3">
+        <v>43172</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="F33" s="2"/>
       <c r="H33" s="2"/>
-      <c r="J33" s="10"/>
+      <c r="I33" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>133</v>
+      </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>4</v>
@@ -1609,19 +1763,20 @@
       <c r="E34" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="F34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
+      </c>
+      <c r="J34" s="13" t="s">
+        <v>135</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>4</v>
@@ -1635,19 +1790,20 @@
       <c r="E35" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="F35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
+      </c>
+      <c r="J35" s="13" t="s">
+        <v>135</v>
       </c>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>4</v>
@@ -1665,15 +1821,15 @@
         <v>22</v>
       </c>
       <c r="H36" s="2"/>
-      <c r="I36" s="12" t="s">
-        <v>118</v>
+      <c r="I36" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>4</v>
@@ -1692,14 +1848,14 @@
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>4</v>
@@ -1711,12 +1867,18 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="H38" s="2"/>
+      <c r="I38" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>130</v>
+      </c>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>4</v>
@@ -1728,12 +1890,18 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="H39" s="2"/>
+      <c r="I39" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="J39" s="12" t="s">
+        <v>138</v>
+      </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>4</v>
@@ -1752,17 +1920,14 @@
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>4</v>
@@ -1781,14 +1946,14 @@
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>4</v>
@@ -1800,12 +1965,18 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="H42" s="2"/>
+      <c r="I42" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="J42" s="12" t="s">
+        <v>116</v>
+      </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>4</v>
@@ -1819,22 +1990,20 @@
       <c r="E43" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="F43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="J43" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
+      </c>
+      <c r="J43" s="13" t="s">
+        <v>137</v>
       </c>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>4</v>
@@ -1848,19 +2017,20 @@
       <c r="E44" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="F44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
+      </c>
+      <c r="J44" s="13" t="s">
+        <v>135</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>4</v>
@@ -1874,12 +2044,13 @@
       <c r="E45" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="F45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="J45" s="13" t="s">
+        <v>135</v>
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
@@ -1894,12 +2065,12 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C47" s="3">
         <v>43112</v>
@@ -1912,15 +2083,18 @@
       <c r="I47" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="J47" s="12" t="s">
+        <v>129</v>
+      </c>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -1931,10 +2105,10 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C49" s="3">
         <v>43111</v>
@@ -1952,10 +2126,10 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C50" s="3">
         <v>43112</v>
@@ -1971,10 +2145,10 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C51" s="3">
         <v>43131</v>
@@ -1997,10 +2171,10 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C52" s="3">
         <v>43112</v>
@@ -2016,10 +2190,10 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C53" s="3">
         <v>43112</v>
@@ -2040,10 +2214,10 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="2"/>
@@ -2054,10 +2228,10 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C55" s="3">
         <v>43112</v>
@@ -2077,10 +2251,10 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C56" s="3">
         <v>43112</v>

</xml_diff>

<commit_message>
updates from latest round of outreach to states
</commit_message>
<xml_diff>
--- a/#State Mapping Status.xlsx
+++ b/#State Mapping Status.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="145">
   <si>
     <t>State</t>
   </si>
@@ -401,9 +401,6 @@
     <t>Michael Lawlor</t>
   </si>
   <si>
-    <t>Lisa Seymour</t>
-  </si>
-  <si>
     <t>Chris Young</t>
   </si>
   <si>
@@ -449,9 +446,6 @@
     <t>Cheryl Payton</t>
   </si>
   <si>
-    <t>Mike contacted on 3/15</t>
-  </si>
-  <si>
     <t>3/15/18 Andrew talking to Matt</t>
   </si>
   <si>
@@ -462,6 +456,15 @@
   </si>
   <si>
     <t>Becki contacted Mannone Butler (SEARCH member) and Ms. Butler is following up on the request</t>
+  </si>
+  <si>
+    <t>Mike contacted on 3/15, need to create mapping</t>
+  </si>
+  <si>
+    <t>David Elwood</t>
+  </si>
+  <si>
+    <t>Mark conntaced on 3/13, Mr. Elwood responded with an example tool - 3/16 - Mike asked for tables</t>
   </si>
 </sst>
 </file>
@@ -885,7 +888,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J48" sqref="J48"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -958,7 +961,7 @@
         <v>89</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -1012,7 +1015,7 @@
         <v>120</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -1067,7 +1070,7 @@
         <v>107</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -1091,7 +1094,7 @@
         <v>121</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -1115,7 +1118,7 @@
         <v>122</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1136,10 +1139,10 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="4" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -1181,16 +1184,20 @@
       <c r="C11" s="3">
         <v>43102</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="2"/>
+      <c r="D11" s="3">
+        <v>43540</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>142</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -1210,10 +1217,10 @@
       <c r="F12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="J12" s="12" t="s">
         <v>124</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>125</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -1242,7 +1249,7 @@
         <v>104</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -1269,7 +1276,7 @@
         <v>82</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -1296,7 +1303,7 @@
         <v>84</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -1378,7 +1385,7 @@
         <v>105</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -1401,7 +1408,7 @@
         <v>112</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -1428,7 +1435,7 @@
         <v>108</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -1451,7 +1458,7 @@
         <v>119</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -1503,7 +1510,7 @@
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
@@ -1530,7 +1537,7 @@
         <v>100</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
@@ -1635,7 +1642,7 @@
         <v>118</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -1664,7 +1671,7 @@
         <v>117</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
@@ -1720,7 +1727,7 @@
         <v>93</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
@@ -1776,7 +1783,7 @@
         <v>116</v>
       </c>
       <c r="J33" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -1803,7 +1810,7 @@
         <v>110</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
@@ -1830,7 +1837,7 @@
         <v>92</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
@@ -1905,7 +1912,7 @@
         <v>115</v>
       </c>
       <c r="J38" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
@@ -1928,7 +1935,7 @@
         <v>114</v>
       </c>
       <c r="J39" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
@@ -2003,7 +2010,7 @@
         <v>113</v>
       </c>
       <c r="J42" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
@@ -2030,7 +2037,7 @@
         <v>102</v>
       </c>
       <c r="J43" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
@@ -2057,7 +2064,7 @@
         <v>83</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
@@ -2084,7 +2091,7 @@
         <v>86</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
@@ -2115,10 +2122,10 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J47" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>

</xml_diff>